<commit_message>
Add 0005 and update BGM
</commit_message>
<xml_diff>
--- a/gallery.xlsx
+++ b/gallery.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -84,6 +84,42 @@
   </si>
   <si>
     <t>26.02.28</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>断面構造,生体マシン,移動オフィス</t>
+  </si>
+  <si>
+    <t>殻の中の定時業務</t>
+  </si>
+  <si>
+    <t>26.03.01</t>
+  </si>
+  <si>
+    <t>さあ 今日は仕事を始めよう
+ここは砂漠エリア
+二週間の滞在だ
+最初は乾いた風に戸惑うが
+そのうち慣れる
+ぼちぼちやればいい
+食料は一階の池にある
+あの水槽の魚だ
+天日干しにするか
+新鮮なら刺身にして
+夕日を眺めながらビールでもやろう
+巨大な殻の内側で
+今日も各部署が動き出す
+カタカタと低い送風音
+おや
+ドクン
+ドクンと床の奥から心臓音
+ああ 彼が目覚めている
+この施設は機械ではない
+生き物だ
+うん
+今日も「正常に異常」</t>
   </si>
 </sst>
 </file>
@@ -352,6 +388,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="5" max="5" width="117.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -539,11 +578,21 @@
       <c r="Y5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>

</xml_diff>